<commit_message>
Asignacion de trabajo (Gabo)
</commit_message>
<xml_diff>
--- a/Grupo de Trabajo.xlsx
+++ b/Grupo de Trabajo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Hugo</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Que Realizó</t>
+  </si>
+  <si>
+    <t>EDT</t>
   </si>
 </sst>
 </file>
@@ -473,17 +476,17 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -497,7 +500,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -509,7 +512,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -521,11 +524,13 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -533,7 +538,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Verificacion de mock up
</commit_message>
<xml_diff>
--- a/Grupo de Trabajo.xlsx
+++ b/Grupo de Trabajo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Hugo</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>EDT</t>
+  </si>
+  <si>
+    <t>UML</t>
   </si>
 </sst>
 </file>
@@ -476,17 +479,17 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -500,7 +503,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +515,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -524,7 +527,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -538,11 +541,13 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>

</xml_diff>